<commit_message>
Use topic.slug and correct test for taxonomy topic ordering
</commit_message>
<xml_diff>
--- a/indigo_app/tests/xlsx_exporter/taxonomies_output_expected.xlsx
+++ b/indigo_app/tests/xlsx_exporter/taxonomies_output_expected.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/coding/laws.africa/indigo/indigo_app/tests/xlsx_exporter/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1EE314-5611-B240-B147-928EAA649CE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="22020" windowHeight="12620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Works" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -160,9 +166,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>lawsafrica-subjects:People and Work/Communications, :Fun stuff</t>
-  </si>
-  <si>
     <t>/akn/za/act/2020/3</t>
   </si>
   <si>
@@ -182,16 +185,19 @@
   </si>
   <si>
     <t>/akn/za/act/2020/4 - Four</t>
+  </si>
+  <si>
+    <t>:Fun stuff, lawsafrica-subjects:People and Work/Communications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +235,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -275,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,9 +321,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,6 +373,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -516,14 +566,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="81.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -658,7 +713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -692,7 +747,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -713,28 +768,28 @@
         <v>44013</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="U4" s="1"/>
       <c r="AC4" t="s">
         <v>38</v>
       </c>
       <c r="AD4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE4" t="s">
         <v>49</v>
       </c>
-      <c r="AE4" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
         <v>51</v>
-      </c>
-      <c r="F5" t="s">
-        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -747,17 +802,17 @@
         <v>44013</v>
       </c>
       <c r="N5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U5" s="1"/>
       <c r="AC5" t="s">
         <v>38</v>
       </c>
       <c r="AD5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE5" t="s">
         <v>54</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>